<commit_message>
graph added in excel files
</commit_message>
<xml_diff>
--- a/Database Fixed/database-fixed-tests/database-fixed-results.xlsx
+++ b/Database Fixed/database-fixed-tests/database-fixed-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarthak.sonagara/Desktop/FINAL PROJECT/Database Fixed/database-fixed-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDF05D2-3C4E-7A48-9C77-60BF5016C7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EE060F-FE3F-254B-A0F2-BAD997A17ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{FF6EBF89-A5B3-F84A-A80F-83D66E3451E5}"/>
   </bookViews>
@@ -153,6 +153,2300 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> time taken to serve a request</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Synchronous</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.8216660148611603E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80424642110342603</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61321853882286503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63609994402320402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80007040619574499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FAD9-0445-B4D3-B62EC35805B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Reactive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.5580077091678605E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77639751552795</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7098108949150199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6197212616577499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3371153974504399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FAD9-0445-B4D3-B62EC35805B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="809013168"/>
+        <c:axId val="299365296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="809013168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of concurrent</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> requests</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299365296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="299365296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="809013168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Throughput</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Synchronous</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.8216660148611603E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80424642110342603</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61321853882286503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63609994402320402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80007040619574499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-994F-294B-950F-E7F99F63DAFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Reactive</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.5580077091678605E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77639751552795</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7098108949150199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6197212616577499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3371153974504399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-994F-294B-950F-E7F99F63DAFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="809013168"/>
+        <c:axId val="299365296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="809013168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of concurrent</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> requests</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299365296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="299365296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Reeuests/second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="809013168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>601082</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>166600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>203516</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38496</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BBA20C8-D345-106F-5376-A6E77BE5A9D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47329</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>189317</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>478025</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>61213</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B58A8719-4C4D-DE48-82EB-937EAEA72B66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,10 +2746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60157135-3E1A-C448-BEB0-13D658116DDB}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +2757,7 @@
     <col min="7" max="7" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,13 +2792,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -539,7 +2833,7 @@
         <v>1019786</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -574,7 +2868,7 @@
         <v>1019786</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -609,7 +2903,7 @@
         <v>1019786</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -644,7 +2938,7 @@
         <v>1019786</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -679,13 +2973,13 @@
         <v>1019786</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -720,7 +3014,7 @@
         <v>1020876</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -754,11 +3048,8 @@
       <c r="K10">
         <v>1020876</v>
       </c>
-      <c r="O10">
-        <v>1000</v>
-      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -793,7 +3084,7 @@
         <v>1020876</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -828,7 +3119,7 @@
         <v>1020876</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -865,5 +3156,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>